<commit_message>
Protocol updata : JogJoint
</commit_message>
<xml_diff>
--- a/PROTOCOL.xlsx
+++ b/PROTOCOL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Module8-9-G7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studio\Module8-9-G7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0991520-B349-4B98-8D3B-3AF8DC50C645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BB38A9-B0C3-48F9-8438-0455DE7399E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27000" yWindow="4845" windowWidth="21600" windowHeight="11430" xr2:uid="{0682010B-CC33-45C9-8DE5-E0BDC4292845}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0682010B-CC33-45C9-8DE5-E0BDC4292845}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="136">
   <si>
     <t>Param1</t>
   </si>
@@ -725,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -850,6 +850,51 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -859,24 +904,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -886,9 +913,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -907,32 +931,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1250,41 +1253,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF5F891-B16F-42AC-96EE-2A8EB25FF4A2}">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19.44140625" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="21.88671875" customWidth="1"/>
-    <col min="15" max="15" width="18.5546875" customWidth="1"/>
-    <col min="16" max="16" width="14.21875" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" customWidth="1"/>
-    <col min="18" max="18" width="14.21875" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
       <c r="H1" s="34"/>
@@ -1302,12 +1304,12 @@
       <c r="T1" s="34"/>
       <c r="U1" s="36"/>
     </row>
-    <row r="2" spans="1:21" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="82"/>
+      <c r="C2" s="63"/>
       <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1361,7 +1363,7 @@
       </c>
       <c r="U2" s="36"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="2">
         <v>1</v>
@@ -1418,7 +1420,7 @@
       <c r="T3" s="4"/>
       <c r="U3" s="36"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="2">
         <v>2</v>
@@ -1475,7 +1477,7 @@
       <c r="T4" s="4"/>
       <c r="U4" s="36"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="2">
         <v>3</v>
@@ -1532,7 +1534,7 @@
       <c r="T5" s="4"/>
       <c r="U5" s="36"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="2">
         <v>4</v>
@@ -1589,7 +1591,7 @@
       <c r="T6" s="4"/>
       <c r="U6" s="36"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="2">
         <v>5</v>
@@ -1646,7 +1648,7 @@
       <c r="T7" s="4"/>
       <c r="U7" s="36"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="6">
         <v>6</v>
@@ -1703,7 +1705,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="36"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="22">
         <v>7</v>
@@ -1760,12 +1762,12 @@
       <c r="T9" s="3"/>
       <c r="U9" s="36"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="84"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="37"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
@@ -1785,7 +1787,7 @@
       <c r="T10" s="34"/>
       <c r="U10" s="36"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -1808,13 +1810,13 @@
       <c r="T11" s="34"/>
       <c r="U11" s="36"/>
     </row>
-    <row r="12" spans="1:21" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34"/>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
       <c r="E12" s="10" t="s">
         <v>53</v>
       </c>
@@ -1839,10 +1841,10 @@
       <c r="L12" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M12" s="85" t="s">
+      <c r="M12" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="N12" s="85"/>
+      <c r="N12" s="65"/>
       <c r="O12" s="34"/>
       <c r="P12" s="34"/>
       <c r="Q12" s="34"/>
@@ -1851,7 +1853,7 @@
       <c r="T12" s="34"/>
       <c r="U12" s="36"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="34"/>
       <c r="B13" s="18">
         <v>1</v>
@@ -1862,11 +1864,11 @@
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="63">
-        <v>0</v>
-      </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="65"/>
+      <c r="E13" s="69">
+        <v>0</v>
+      </c>
+      <c r="F13" s="70"/>
+      <c r="G13" s="71"/>
       <c r="H13" s="8" t="s">
         <v>87</v>
       </c>
@@ -1882,8 +1884,8 @@
       <c r="L13" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="M13" s="86"/>
-      <c r="N13" s="87"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="68"/>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
@@ -1892,7 +1894,7 @@
       <c r="T13" s="34"/>
       <c r="U13" s="36"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="34"/>
       <c r="B14" s="18">
         <v>3</v>
@@ -1903,14 +1905,12 @@
       <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="66">
-        <v>0</v>
-      </c>
-      <c r="F14" s="68"/>
-      <c r="G14" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="12" t="s">
+      <c r="E14" s="72">
+        <v>0</v>
+      </c>
+      <c r="F14" s="73"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="88" t="s">
         <v>77</v>
       </c>
       <c r="I14" s="15" t="s">
@@ -1939,7 +1939,7 @@
       <c r="T14" s="34"/>
       <c r="U14" s="36"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="18">
         <v>4</v>
@@ -1950,11 +1950,11 @@
       <c r="D15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="66">
-        <v>0</v>
-      </c>
-      <c r="F15" s="67"/>
-      <c r="G15" s="68"/>
+      <c r="E15" s="72">
+        <v>0</v>
+      </c>
+      <c r="F15" s="73"/>
+      <c r="G15" s="74"/>
       <c r="H15" s="14" t="s">
         <v>85</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="T15" s="34"/>
       <c r="U15" s="36"/>
     </row>
-    <row r="16" spans="1:21" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
@@ -2007,14 +2007,14 @@
       <c r="T16" s="35"/>
       <c r="U16" s="38"/>
     </row>
-    <row r="17" spans="1:21" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
@@ -2032,12 +2032,12 @@
       <c r="T17" s="34"/>
       <c r="U17" s="31"/>
     </row>
-    <row r="18" spans="1:21" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="17" t="s">
         <v>3</v>
       </c>
@@ -2091,7 +2091,7 @@
       </c>
       <c r="U18" s="36"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
       <c r="B19" s="18">
         <v>1</v>
@@ -2108,35 +2108,35 @@
       <c r="F19" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="79" t="s">
+      <c r="G19" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="H19" s="80"/>
-      <c r="I19" s="79" t="s">
+      <c r="H19" s="61"/>
+      <c r="I19" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="80"/>
-      <c r="K19" s="79" t="s">
+      <c r="J19" s="61"/>
+      <c r="K19" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="80"/>
-      <c r="M19" s="79" t="s">
+      <c r="L19" s="61"/>
+      <c r="M19" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="N19" s="80"/>
-      <c r="O19" s="79" t="s">
+      <c r="N19" s="61"/>
+      <c r="O19" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="P19" s="80"/>
-      <c r="Q19" s="79" t="s">
+      <c r="P19" s="61"/>
+      <c r="Q19" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="R19" s="80"/>
+      <c r="R19" s="61"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="36"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
       <c r="B20" s="18">
         <v>3</v>
@@ -2153,10 +2153,10 @@
       <c r="F20" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="79" t="s">
+      <c r="G20" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="H20" s="80"/>
+      <c r="H20" s="61"/>
       <c r="I20" s="26"/>
       <c r="J20" s="26"/>
       <c r="K20" s="26"/>
@@ -2171,7 +2171,7 @@
       <c r="T20" s="4"/>
       <c r="U20" s="36"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="34"/>
       <c r="B21" s="18">
         <v>4</v>
@@ -2188,22 +2188,22 @@
       <c r="F21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="73" t="s">
+      <c r="G21" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="H21" s="74"/>
-      <c r="I21" s="73" t="s">
+      <c r="H21" s="82"/>
+      <c r="I21" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="J21" s="74"/>
-      <c r="K21" s="73" t="s">
+      <c r="J21" s="82"/>
+      <c r="K21" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="L21" s="74"/>
-      <c r="M21" s="73" t="s">
+      <c r="L21" s="82"/>
+      <c r="M21" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="N21" s="74"/>
+      <c r="N21" s="82"/>
       <c r="O21" s="26" t="s">
         <v>35</v>
       </c>
@@ -2220,7 +2220,7 @@
       <c r="T21" s="4"/>
       <c r="U21" s="36"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="34"/>
       <c r="B22" s="18">
         <v>5</v>
@@ -2237,14 +2237,14 @@
       <c r="F22" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="75"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="76"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="84"/>
       <c r="O22" s="26" t="s">
         <v>35</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="T22" s="4"/>
       <c r="U22" s="36"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="34"/>
       <c r="B23" s="6">
         <v>6</v>
@@ -2278,14 +2278,14 @@
       <c r="F23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="77"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="78"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="85"/>
+      <c r="N23" s="86"/>
       <c r="O23" s="26" t="s">
         <v>44</v>
       </c>
@@ -2302,7 +2302,7 @@
       <c r="T23" s="3"/>
       <c r="U23" s="36"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="34"/>
       <c r="B24" s="6">
         <v>7</v>
@@ -2359,12 +2359,12 @@
       <c r="T24" s="3"/>
       <c r="U24" s="36"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="83"/>
+      <c r="C25" s="87"/>
       <c r="D25" s="37"/>
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
@@ -2384,7 +2384,7 @@
       <c r="T25" s="34"/>
       <c r="U25" s="36"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
@@ -2407,7 +2407,7 @@
       <c r="T26" s="34"/>
       <c r="U26" s="36"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -2430,7 +2430,7 @@
       <c r="T27" s="34"/>
       <c r="U27" s="36"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -2457,7 +2457,7 @@
       <c r="T28" s="34"/>
       <c r="U28" s="36"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
@@ -2506,11 +2506,11 @@
       <c r="T29" s="52"/>
       <c r="U29" s="36"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="34"/>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
-      <c r="D30" s="61" t="s">
+      <c r="D30" s="76" t="s">
         <v>105</v>
       </c>
       <c r="E30" s="32" t="s">
@@ -2549,17 +2549,17 @@
       <c r="T30" s="34"/>
       <c r="U30" s="36"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
       <c r="B31" s="34"/>
       <c r="C31" s="34"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="69" t="s">
+      <c r="D31" s="77"/>
+      <c r="E31" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="71"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="80"/>
       <c r="I31" s="34"/>
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
@@ -2574,7 +2574,7 @@
       <c r="T31" s="34"/>
       <c r="U31" s="36"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="34"/>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
@@ -2597,7 +2597,7 @@
       <c r="T32" s="34"/>
       <c r="U32" s="36"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="34"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
@@ -2620,7 +2620,7 @@
       <c r="T33" s="34"/>
       <c r="U33" s="36"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
       <c r="C34" s="34"/>
@@ -2647,7 +2647,7 @@
       <c r="T34" s="34"/>
       <c r="U34" s="36"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
       <c r="C35" s="34"/>
@@ -2686,7 +2686,7 @@
       <c r="T35" s="50"/>
       <c r="U35" s="33"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
       <c r="C36" s="34"/>
@@ -2700,7 +2700,7 @@
       <c r="K36" s="34"/>
       <c r="L36" s="34"/>
       <c r="M36" s="34"/>
-      <c r="N36" s="61" t="s">
+      <c r="N36" s="76" t="s">
         <v>133</v>
       </c>
       <c r="O36" s="56" t="s">
@@ -2713,13 +2713,13 @@
       <c r="T36" s="34"/>
       <c r="U36" s="36"/>
     </row>
-    <row r="37" spans="1:21" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
-      <c r="B37" s="72" t="s">
+      <c r="B37" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
       <c r="E37" s="10" t="s">
         <v>53</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>60</v>
       </c>
       <c r="M37" s="39"/>
-      <c r="N37" s="62"/>
+      <c r="N37" s="77"/>
       <c r="O37" s="56" t="s">
         <v>135</v>
       </c>
@@ -2756,7 +2756,7 @@
       <c r="T37" s="34"/>
       <c r="U37" s="36"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="34"/>
       <c r="B38" s="18">
         <v>1</v>
@@ -2767,18 +2767,18 @@
       <c r="D38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="63" t="s">
+      <c r="E38" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="F38" s="64"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="66" t="s">
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="J38" s="67"/>
-      <c r="K38" s="67"/>
-      <c r="L38" s="68"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="74"/>
       <c r="M38" s="55"/>
       <c r="N38" s="58"/>
       <c r="O38" s="34"/>
@@ -2789,7 +2789,7 @@
       <c r="T38" s="34"/>
       <c r="U38" s="36"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
       <c r="B39" s="18"/>
       <c r="C39" s="28"/>
@@ -2812,7 +2812,7 @@
       <c r="T39" s="34"/>
       <c r="U39" s="36"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
       <c r="B40" s="18"/>
       <c r="C40" s="28"/>
@@ -2835,7 +2835,7 @@
       <c r="T40" s="34"/>
       <c r="U40" s="36"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" s="35"/>
       <c r="C41" s="35"/>
@@ -2860,19 +2860,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="N36:N37"/>
@@ -2889,6 +2876,19 @@
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="B25:C25"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commmit new low level
</commit_message>
<xml_diff>
--- a/PROTOCOL.xlsx
+++ b/PROTOCOL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Module8-9-G7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5E25C8-A1D2-4DF8-9D17-4F973B361F40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12692008-A44F-462F-BA97-6D3F95A38D32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{0682010B-CC33-45C9-8DE5-E0BDC4292845}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{0682010B-CC33-45C9-8DE5-E0BDC4292845}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -944,6 +944,54 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -965,58 +1013,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1335,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF5F891-B16F-42AC-96EE-2A8EB25FF4A2}">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,12 +1365,12 @@
   <sheetData>
     <row r="1" spans="1:26" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
@@ -1395,10 +1395,10 @@
     </row>
     <row r="2" spans="1:26" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="73"/>
+      <c r="C2" s="89"/>
       <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1893,10 +1893,10 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="74"/>
+      <c r="C10" s="90"/>
       <c r="D10" s="33"/>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
@@ -1951,11 +1951,11 @@
     </row>
     <row r="12" spans="1:26" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
       <c r="E12" s="9" t="s">
         <v>44</v>
       </c>
@@ -1980,10 +1980,10 @@
       <c r="L12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="75" t="s">
+      <c r="M12" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="N12" s="75"/>
+      <c r="N12" s="91"/>
       <c r="O12" s="30"/>
       <c r="P12" s="30"/>
       <c r="Q12" s="30"/>
@@ -2032,8 +2032,8 @@
       <c r="L13" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="M13" s="77"/>
-      <c r="N13" s="78"/>
+      <c r="M13" s="92"/>
+      <c r="N13" s="93"/>
       <c r="O13" s="30"/>
       <c r="P13" s="30"/>
       <c r="Q13" s="30"/>
@@ -2058,11 +2058,11 @@
       <c r="D14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="81">
-        <v>0</v>
-      </c>
-      <c r="F14" s="82"/>
-      <c r="G14" s="83"/>
+      <c r="E14" s="75">
+        <v>0</v>
+      </c>
+      <c r="F14" s="76"/>
+      <c r="G14" s="77"/>
       <c r="H14" s="12" t="s">
         <v>73</v>
       </c>
@@ -2108,11 +2108,11 @@
       <c r="D15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="81">
-        <v>0</v>
-      </c>
-      <c r="F15" s="82"/>
-      <c r="G15" s="83"/>
+      <c r="E15" s="75">
+        <v>0</v>
+      </c>
+      <c r="F15" s="76"/>
+      <c r="G15" s="77"/>
       <c r="H15" s="11" t="s">
         <v>73</v>
       </c>
@@ -2177,12 +2177,12 @@
     </row>
     <row r="17" spans="1:26" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
@@ -2207,10 +2207,10 @@
     </row>
     <row r="18" spans="1:26" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="73"/>
+      <c r="C18" s="89"/>
       <c r="D18" s="14" t="s">
         <v>3</v>
       </c>
@@ -2294,38 +2294,38 @@
       <c r="F19" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="79" t="s">
+      <c r="G19" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="H19" s="80"/>
-      <c r="I19" s="79" t="s">
+      <c r="H19" s="83"/>
+      <c r="I19" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="J19" s="80"/>
-      <c r="K19" s="79" t="s">
+      <c r="J19" s="83"/>
+      <c r="K19" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="L19" s="80"/>
-      <c r="M19" s="79" t="s">
+      <c r="L19" s="83"/>
+      <c r="M19" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="N19" s="80"/>
-      <c r="O19" s="79" t="s">
+      <c r="N19" s="83"/>
+      <c r="O19" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="P19" s="80"/>
-      <c r="Q19" s="79" t="s">
+      <c r="P19" s="83"/>
+      <c r="Q19" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="R19" s="80"/>
-      <c r="S19" s="69" t="s">
+      <c r="R19" s="83"/>
+      <c r="S19" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="T19" s="70"/>
-      <c r="U19" s="71" t="s">
+      <c r="T19" s="86"/>
+      <c r="U19" s="87" t="s">
         <v>142</v>
       </c>
-      <c r="V19" s="71"/>
+      <c r="V19" s="87"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="30"/>
@@ -2579,10 +2579,10 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
-      <c r="B25" s="93" t="s">
+      <c r="B25" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="93"/>
+      <c r="C25" s="84"/>
       <c r="D25" s="33"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
@@ -2767,7 +2767,7 @@
       <c r="A30" s="30"/>
       <c r="B30" s="30"/>
       <c r="C30" s="30"/>
-      <c r="D30" s="85" t="s">
+      <c r="D30" s="70" t="s">
         <v>92</v>
       </c>
       <c r="E30" s="29" t="s">
@@ -2823,13 +2823,13 @@
       <c r="A31" s="30"/>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="90" t="s">
+      <c r="D31" s="71"/>
+      <c r="E31" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="92"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="80"/>
       <c r="I31" s="30"/>
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
@@ -3035,7 +3035,7 @@
       <c r="K36" s="30"/>
       <c r="L36" s="30"/>
       <c r="M36" s="30"/>
-      <c r="N36" s="85" t="s">
+      <c r="N36" s="70" t="s">
         <v>120</v>
       </c>
       <c r="O36" s="51" t="s">
@@ -3063,11 +3063,11 @@
     </row>
     <row r="37" spans="1:26" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30"/>
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81"/>
       <c r="E37" s="9" t="s">
         <v>44</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>51</v>
       </c>
       <c r="M37" s="35"/>
-      <c r="N37" s="86"/>
+      <c r="N37" s="71"/>
       <c r="O37" s="51" t="s">
         <v>122</v>
       </c>
@@ -3120,18 +3120,18 @@
       <c r="D38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="87" t="s">
+      <c r="E38" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="F38" s="88"/>
-      <c r="G38" s="88"/>
-      <c r="H38" s="89"/>
-      <c r="I38" s="81" t="s">
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="J38" s="82"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="83"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="77"/>
       <c r="M38" s="50"/>
       <c r="N38" s="53"/>
       <c r="O38" s="30"/>
@@ -3233,6 +3233,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
     <mergeCell ref="K20:L23"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B17:E17"/>
@@ -3248,19 +3261,6 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="M20:N23"/>
     <mergeCell ref="G20:H23"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
     <mergeCell ref="I20:J23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>